<commit_message>
Next buttons in new Study foirm sites; user specific dropdowns in all forms;
</commit_message>
<xml_diff>
--- a/other_data/Lab_analytes_EuBIVAS.xlsx
+++ b/other_data/Lab_analytes_EuBIVAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janne\PycharmProjects\stability_calculator\other_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janne Lokal\PycharmProjects\StabilityCalc\other_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A547B7-6608-41EE-8190-981C4ED2F5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5A4187-6913-4206-BC07-861909DA827D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="-18120" windowWidth="28110" windowHeight="18240" xr2:uid="{5B6BD98A-A6B5-4370-BDC7-3BB7C6471867}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B6BD98A-A6B5-4370-BDC7-3BB7C6471867}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF93899-C357-4A42-9CD7-642802BEC722}">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1655,6 +1655,9 @@
       <c r="E47">
         <v>8.9</v>
       </c>
+      <c r="F47">
+        <v>8</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">

</xml_diff>